<commit_message>
FINAL com bug de duplicidade corrigido.
</commit_message>
<xml_diff>
--- a/dados_envio.xlsx
+++ b/dados_envio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I9 BR Group\Desktop\Projetos Desenvolvimento\Relatorio Suzano\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I9 BR Group\Desktop\Projetos Desenvolvimento\Nodrop_NOVOt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9415DE-D73C-4A1A-B150-8C86AF37C426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C55AA4C-A8C2-42ED-B3AD-88F427DF7BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>cribs-interval</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>pedrohique@hotmail.com, backoffice@i9brgroup.com.br, backoffice2@i9brgroup.com.br</t>
+  </si>
+  <si>
+    <t>220-224</t>
+  </si>
+  <si>
+    <t>Suzano Imperatriz</t>
+  </si>
+  <si>
+    <t>Brascabos</t>
   </si>
 </sst>
 </file>
@@ -423,7 +432,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,6 +568,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
     </row>

</xml_diff>